<commit_message>
Updates - searching, logging & README
</commit_message>
<xml_diff>
--- a/RS/Files/store_info.xlsx
+++ b/RS/Files/store_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brad6\Desktop\Code Projects\Data\Store_Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC4860D-EAB3-44CE-A787-DD6DAC5F6FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF653DD7-E355-4A7C-843A-1E33F0FFD9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{147BDEBE-6DAD-421D-8B7E-61774E94A83F}"/>
   </bookViews>
@@ -476,22 +476,22 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>store_name</t>
-  </si>
-  <si>
-    <t>store_address</t>
-  </si>
-  <si>
-    <t>store_postcode</t>
-  </si>
-  <si>
-    <t>kms</t>
-  </si>
-  <si>
-    <t>tail_lift</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Store Name</t>
+  </si>
+  <si>
+    <t>Store Address</t>
+  </si>
+  <si>
+    <t>Store Postcode</t>
+  </si>
+  <si>
+    <t>Kilometers</t>
+  </si>
+  <si>
+    <t>Tail Lift</t>
   </si>
 </sst>
 </file>

</xml_diff>